<commit_message>
user story#2002 : testing
</commit_message>
<xml_diff>
--- a/DataTables/Book7.xlsx
+++ b/DataTables/Book7.xlsx
@@ -39,10 +39,10 @@
     <t>e</t>
   </si>
   <si>
-    <t>f</t>
-  </si>
-  <si>
-    <t>d</t>
+    <t>d2</t>
+  </si>
+  <si>
+    <t>f2</t>
   </si>
 </sst>
 </file>
@@ -364,7 +364,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -382,7 +382,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -390,7 +390,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
defect #3002:sksk , user story #2003: anothere tesrl
</commit_message>
<xml_diff>
--- a/DataTables/Book7.xlsx
+++ b/DataTables/Book7.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
   <si>
     <t>a</t>
   </si>
@@ -42,13 +42,10 @@
     <t>d2</t>
   </si>
   <si>
-    <t>f2</t>
-  </si>
-  <si>
     <t>g</t>
   </si>
   <si>
-    <t>g4</t>
+    <t>f3</t>
   </si>
 </sst>
 </file>
@@ -370,7 +367,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -396,15 +393,15 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
defect #3001: second commit
</commit_message>
<xml_diff>
--- a/DataTables/Book7.xlsx
+++ b/DataTables/Book7.xlsx
@@ -39,13 +39,13 @@
     <t>e</t>
   </si>
   <si>
-    <t>d2</t>
-  </si>
-  <si>
     <t>g</t>
   </si>
   <si>
     <t>f3</t>
+  </si>
+  <si>
+    <t>d</t>
   </si>
 </sst>
 </file>
@@ -367,7 +367,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -385,7 +385,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -393,15 +393,15 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>